<commit_message>
result tables are done
</commit_message>
<xml_diff>
--- a/model/data/results/TESTING RESULTS RLKG.xlsx
+++ b/model/data/results/TESTING RESULTS RLKG.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migberbay\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\migberbay\RL-KG\model\data\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86832F8A-3146-4337-9777-F047423B93D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7696EF06-811B-44D6-999C-E636398F9DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{B4182266-BC67-4EA4-AAE0-998703FC7B9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4182266-BC67-4EA4-AAE0-998703FC7B9B}"/>
   </bookViews>
   <sheets>
     <sheet name="WN18 self" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
   <si>
     <t>Relation Name</t>
   </si>
@@ -49,28 +49,7 @@
     <t>derivationally_related_from</t>
   </si>
   <si>
-    <t>has_part</t>
-  </si>
-  <si>
-    <t>hypernym</t>
-  </si>
-  <si>
-    <t>instance_hypernym</t>
-  </si>
-  <si>
-    <t>member_meronym</t>
-  </si>
-  <si>
-    <t>member_of_domain_region</t>
-  </si>
-  <si>
-    <t>member_of_domain_usage</t>
-  </si>
-  <si>
     <t>similar_to</t>
-  </si>
-  <si>
-    <t>synset_domain_topic_of</t>
   </si>
   <si>
     <t>verb_group</t>
@@ -152,7 +131,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +143,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,9 +177,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -508,66 +497,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE24F8F-950E-4D73-9EA5-1F051D6635D7}">
-  <dimension ref="B4:J16"/>
+  <dimension ref="B4:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.88671875" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.1666</v>
+        <v>0.64659999999999995</v>
       </c>
       <c r="D5">
-        <v>0.41499999999999998</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="E5">
-        <v>0.58499999999999996</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="F5">
-        <v>0.83520000000000005</v>
+        <v>0.93520000000000003</v>
       </c>
       <c r="G5">
-        <v>0.34585761904761803</v>
+        <v>0.74585761904761805</v>
       </c>
       <c r="H5">
         <v>1299</v>
@@ -580,15 +569,15 @@
         <v>259800</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6">
-        <v>0.2258</v>
+        <v>0.58579999999999999</v>
       </c>
       <c r="D6">
-        <v>0.56140000000000001</v>
+        <v>0.65139999999999998</v>
       </c>
       <c r="E6">
         <v>0.74660000000000004</v>
@@ -597,7 +586,7 @@
         <v>0.93340000000000001</v>
       </c>
       <c r="G6">
-        <v>0.437527063492061</v>
+        <v>0.63752706349206101</v>
       </c>
       <c r="H6">
         <v>29715</v>
@@ -606,295 +595,105 @@
         <v>100</v>
       </c>
       <c r="J6">
-        <f t="shared" ref="J6:J16" si="0">(H6*I6)</f>
+        <f t="shared" ref="J6" si="0">(H6*I6)</f>
         <v>2971500</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7">
-        <v>8.8000000000000005E-3</v>
+        <v>0.83079999999999998</v>
       </c>
       <c r="D7">
-        <v>2.1999999999999999E-2</v>
+        <v>0.99560000000000004</v>
       </c>
       <c r="E7">
-        <v>3.78E-2</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>7.6999999999999999E-2</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>2.31140476190476E-2</v>
+        <v>0.90984666666666703</v>
       </c>
       <c r="H7">
-        <v>4816</v>
+        <v>80</v>
       </c>
       <c r="I7">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
-        <v>481600</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+        <f>(H7*I7)</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8">
-        <v>2.1000000000000001E-2</v>
+        <v>0.60940000000000005</v>
       </c>
       <c r="D8">
-        <v>5.5599999999999997E-2</v>
+        <v>0.93459999999999999</v>
       </c>
       <c r="E8">
-        <v>9.1800000000000007E-2</v>
+        <v>0.98939999999999995</v>
       </c>
       <c r="F8">
-        <v>0.17519999999999999</v>
+        <v>0.99980000000000002</v>
       </c>
       <c r="G8">
-        <v>5.4114999999999802E-2</v>
+        <v>0.77185388888889295</v>
       </c>
       <c r="H8">
-        <v>34796</v>
+        <v>1138</v>
       </c>
       <c r="I8">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
-        <v>3479600</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+        <f>(H8*I8)</f>
+        <v>170700</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C9">
-        <v>7.0800000000000002E-2</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="D9">
-        <v>0.2036</v>
+        <v>0.4844</v>
       </c>
       <c r="E9">
-        <v>0.32979999999999998</v>
+        <v>0.52359999999999995</v>
       </c>
       <c r="F9">
-        <v>0.54700000000000004</v>
+        <v>0.66059999999999997</v>
       </c>
       <c r="G9">
-        <v>0.18281325396825401</v>
-      </c>
-      <c r="H9">
-        <v>2921</v>
+        <v>0.44310531746031701</v>
+      </c>
+      <c r="H9" s="3">
+        <v>80798</v>
       </c>
       <c r="I9">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
-        <v>292100</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>1.4E-3</v>
-      </c>
-      <c r="D10">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="E10">
-        <v>9.5999999999999992E-3</v>
-      </c>
-      <c r="F10">
-        <v>1.9199999999999998E-2</v>
-      </c>
-      <c r="G10">
-        <v>5.3845238095238E-3</v>
-      </c>
-      <c r="H10">
-        <v>923</v>
-      </c>
-      <c r="I10">
-        <v>200</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>184600</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="D11">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="E11">
-        <v>6.1999999999999998E-3</v>
-      </c>
-      <c r="F11">
-        <v>1.18E-2</v>
-      </c>
-      <c r="G11">
-        <v>3.0953174603174502E-3</v>
-      </c>
-      <c r="H11">
-        <v>629</v>
-      </c>
-      <c r="I11">
-        <v>200</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>125800</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>1.2200000000000001E-2</v>
-      </c>
-      <c r="D12">
-        <v>2.98E-2</v>
-      </c>
-      <c r="E12">
-        <v>4.5400000000000003E-2</v>
-      </c>
-      <c r="F12">
-        <v>8.8999999999999996E-2</v>
-      </c>
-      <c r="G12">
-        <v>2.87570634920634E-2</v>
-      </c>
-      <c r="H12">
-        <v>7402</v>
-      </c>
-      <c r="I12">
-        <v>100</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>740200</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13">
-        <v>0.83079999999999998</v>
-      </c>
-      <c r="D13">
-        <v>0.99560000000000004</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>0.90984666666666703</v>
-      </c>
-      <c r="H13">
-        <v>80</v>
-      </c>
-      <c r="I13">
-        <v>500</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <v>5.28E-2</v>
-      </c>
-      <c r="D14">
-        <v>0.14660000000000001</v>
-      </c>
-      <c r="E14">
-        <v>0.2326</v>
-      </c>
-      <c r="F14">
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="G14">
-        <v>0.135313809523809</v>
-      </c>
-      <c r="H14">
-        <v>3116</v>
-      </c>
-      <c r="I14">
-        <v>100</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>311600</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15">
-        <v>0.60940000000000005</v>
-      </c>
-      <c r="D15">
-        <v>0.93459999999999999</v>
-      </c>
-      <c r="E15">
-        <v>0.98939999999999995</v>
-      </c>
-      <c r="F15">
-        <v>0.99980000000000002</v>
-      </c>
-      <c r="G15">
-        <v>0.77185388888889295</v>
-      </c>
-      <c r="H15">
-        <v>1138</v>
-      </c>
-      <c r="I15">
-        <v>150</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>170700</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16">
-        <f>SUM(H5:H15)</f>
-        <v>86835</v>
-      </c>
-      <c r="I16">
-        <v>50</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
-        <v>4341750</v>
-      </c>
+        <f>(H9*I9)</f>
+        <v>6059850</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M10" s="2"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -904,6 +703,7 @@
     <hyperlink ref="F4" r:id="rId4" xr:uid="{9DAE7E39-2A63-437F-8AE6-8D8D2ACB2B22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -911,69 +711,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D82D4B-68BF-4307-93EF-011667BAD0F7}">
   <dimension ref="B2:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.109375" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
       <c r="C4">
-        <v>7.6E-3</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="D4">
-        <v>2.7199999999999998E-2</v>
+        <v>0.252</v>
       </c>
       <c r="E4">
-        <v>4.3200000000000002E-2</v>
+        <v>0.315</v>
       </c>
       <c r="F4">
-        <v>8.1199999999999994E-2</v>
+        <v>0.38</v>
       </c>
       <c r="G4">
-        <v>2.4229682539682499E-2</v>
+        <v>0.25679682539688198</v>
       </c>
       <c r="H4">
         <v>7268</v>
@@ -986,24 +786,24 @@
         <v>159896</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>9.1999999999999998E-3</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="D5">
-        <v>2.8799999999999999E-2</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="E5">
-        <v>4.36E-2</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="F5">
-        <v>8.3199999999999996E-2</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="G5">
-        <v>2.57133333333333E-2</v>
+        <v>0.26729682539688199</v>
       </c>
       <c r="H5">
         <v>7268</v>
@@ -1016,24 +816,24 @@
         <v>159896</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>6.4000000000000003E-3</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="D6">
-        <v>2.6800000000000001E-2</v>
+        <v>0.376</v>
       </c>
       <c r="E6">
-        <v>4.0800000000000003E-2</v>
+        <v>0.42299999999999999</v>
       </c>
       <c r="F6">
-        <v>8.4000000000000005E-2</v>
+        <v>0.51600000000000001</v>
       </c>
       <c r="G6">
-        <v>2.33879365079365E-2</v>
+        <v>0.382968253968825</v>
       </c>
       <c r="H6">
         <v>7268</v>
@@ -1046,13 +846,34 @@
         <v>159896</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>0.25</v>
+      </c>
+      <c r="D7">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="E7">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="G7">
+        <v>0.408296825396882</v>
+      </c>
+      <c r="H7">
+        <v>7268</v>
+      </c>
+      <c r="I7">
+        <v>22</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>159896</v>
       </c>
     </row>
   </sheetData>
@@ -1068,77 +889,77 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D4B5C1-BE7A-4F0E-AF51-4C9258E72885}">
-  <dimension ref="B3:L15"/>
+  <dimension ref="B3:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E4">
-        <v>1.32E-2</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="F4">
-        <v>3.2199999999999999E-2</v>
+        <v>0.80420000000000003</v>
       </c>
       <c r="G4">
-        <v>5.3999999999999999E-2</v>
+        <v>0.90800000000000003</v>
       </c>
       <c r="H4">
-        <v>0.104</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="I4">
-        <v>3.2627222222222099E-2</v>
+        <v>0.69086507936550001</v>
       </c>
       <c r="J4">
         <v>230</v>
@@ -1151,30 +972,30 @@
         <v>57500</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E5">
-        <v>1.0999999999999999E-2</v>
+        <v>0.58789999999999998</v>
       </c>
       <c r="F5">
-        <v>3.3599999999999998E-2</v>
+        <v>0.89679999999999993</v>
       </c>
       <c r="G5">
-        <v>5.0999999999999997E-2</v>
+        <v>0.96349999999999991</v>
       </c>
       <c r="H5">
-        <v>0.1038</v>
+        <v>0.98659999999999992</v>
       </c>
       <c r="I5">
-        <v>3.10503174603174E-2</v>
+        <v>0.77109430055000006</v>
       </c>
       <c r="J5">
         <v>230</v>
@@ -1187,30 +1008,30 @@
         <v>57500</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E6">
-        <v>1.04E-2</v>
+        <v>0.5514</v>
       </c>
       <c r="F6">
-        <v>2.6800000000000001E-2</v>
+        <v>0.86899999999999999</v>
       </c>
       <c r="G6">
-        <v>4.6199999999999998E-2</v>
+        <v>0.94739999999999991</v>
       </c>
       <c r="H6">
-        <v>9.3600000000000003E-2</v>
+        <v>0.98319999999999996</v>
       </c>
       <c r="I6">
-        <v>2.7821507936507901E-2</v>
+        <v>0.73348607193651105</v>
       </c>
       <c r="J6">
         <v>230</v>
@@ -1223,30 +1044,30 @@
         <v>57500</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E7">
-        <v>1.9800000000000002E-2</v>
+        <v>0.63379999999999992</v>
       </c>
       <c r="F7">
-        <v>5.7200000000000001E-2</v>
+        <v>0.95299999999999996</v>
       </c>
       <c r="G7">
-        <v>9.7000000000000003E-2</v>
+        <v>0.996</v>
       </c>
       <c r="H7">
-        <v>0.1812</v>
+        <v>0.99919999999999998</v>
       </c>
       <c r="I7">
-        <v>5.51088888888887E-2</v>
+        <v>0.78894821479365507</v>
       </c>
       <c r="J7">
         <v>230</v>
@@ -1259,66 +1080,30 @@
         <v>57500</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8">
-        <v>0.63039999999999996</v>
-      </c>
-      <c r="F8">
-        <v>0.9496</v>
-      </c>
-      <c r="G8">
-        <v>0.99260000000000004</v>
-      </c>
-      <c r="H8">
-        <v>0.99980000000000002</v>
-      </c>
-      <c r="I8">
-        <v>0.78680865079365503</v>
-      </c>
-      <c r="J8">
-        <v>259</v>
-      </c>
-      <c r="K8">
-        <v>250</v>
-      </c>
-      <c r="L8">
-        <f>(J8*K8)</f>
-        <v>64750</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E9">
-        <v>5.7999999999999996E-3</v>
+        <v>0.41039999999999999</v>
       </c>
       <c r="F9">
-        <v>1.38E-2</v>
+        <v>0.76959999999999995</v>
       </c>
       <c r="G9">
-        <v>2.2800000000000001E-2</v>
+        <v>0.87339999999999995</v>
       </c>
       <c r="H9">
-        <v>4.6399999999999997E-2</v>
+        <v>0.91449999999999998</v>
       </c>
       <c r="I9">
-        <v>1.42916666666666E-2</v>
+        <v>0.69086507936550001</v>
       </c>
       <c r="J9">
         <v>259</v>
@@ -1327,34 +1112,34 @@
         <v>250</v>
       </c>
       <c r="L9">
-        <f t="shared" ref="L9:L11" si="1">(J9*K9)</f>
+        <f>(J9*K9)</f>
         <v>64750</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E10">
-        <v>0.54800000000000004</v>
+        <v>0.58450000000000002</v>
       </c>
       <c r="F10">
-        <v>0.91559999999999997</v>
+        <v>0.89339999999999997</v>
       </c>
       <c r="G10">
-        <v>0.98399999999999999</v>
+        <v>0.96009999999999995</v>
       </c>
       <c r="H10">
-        <v>0.99980000000000002</v>
+        <v>0.98319999999999996</v>
       </c>
       <c r="I10">
-        <v>0.73134650793651101</v>
+        <v>0.76895473655000002</v>
       </c>
       <c r="J10">
         <v>259</v>
@@ -1363,34 +1148,34 @@
         <v>250</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="L10:L12" si="1">(J10*K10)</f>
         <v>64750</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E11">
-        <v>6.7400000000000002E-2</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="F11">
-        <v>0.19040000000000001</v>
+        <v>0.86560000000000004</v>
       </c>
       <c r="G11">
-        <v>0.29720000000000002</v>
+        <v>0.94399999999999995</v>
       </c>
       <c r="H11">
-        <v>0.50939999999999996</v>
+        <v>0.9798</v>
       </c>
       <c r="I11">
-        <v>0.17140857142857099</v>
+        <v>0.73134650793651101</v>
       </c>
       <c r="J11">
         <v>259</v>
@@ -1403,102 +1188,66 @@
         <v>64750</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12">
+        <v>0.63039999999999996</v>
+      </c>
+      <c r="F12">
+        <v>0.9496</v>
+      </c>
+      <c r="G12">
+        <v>0.99260000000000004</v>
+      </c>
+      <c r="H12">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="I12">
+        <v>0.78680865079365503</v>
+      </c>
+      <c r="J12">
+        <v>259</v>
+      </c>
+      <c r="K12">
+        <v>250</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>64750</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="F12">
-        <v>0.48720000000000002</v>
-      </c>
-      <c r="G12">
-        <v>0.66539999999999999</v>
-      </c>
-      <c r="H12">
-        <v>0.88919999999999999</v>
-      </c>
-      <c r="I12">
-        <v>0.39354753968253697</v>
-      </c>
-      <c r="J12">
-        <v>773</v>
-      </c>
-      <c r="K12">
-        <v>150</v>
-      </c>
-      <c r="L12">
-        <f>(J12*K12)</f>
-        <v>115950</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13">
-        <v>0.15079999999999999</v>
-      </c>
-      <c r="F13">
-        <v>0.39079999999999998</v>
-      </c>
-      <c r="G13">
-        <v>0.56340000000000001</v>
-      </c>
-      <c r="H13">
-        <v>0.81940000000000002</v>
-      </c>
-      <c r="I13">
-        <v>0.32576539682539501</v>
-      </c>
-      <c r="J13">
-        <v>773</v>
-      </c>
-      <c r="K13">
-        <v>150</v>
-      </c>
-      <c r="L13">
-        <f t="shared" ref="L13:L15" si="2">(J13*K13)</f>
-        <v>115950</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E14">
-        <v>4.3799999999999999E-2</v>
+        <v>0.4093</v>
       </c>
       <c r="F14">
-        <v>0.121</v>
+        <v>0.76849999999999996</v>
       </c>
       <c r="G14">
-        <v>0.19800000000000001</v>
+        <v>0.85709999999999986</v>
       </c>
       <c r="H14">
-        <v>0.34799999999999998</v>
+        <v>0.89819999999999989</v>
       </c>
       <c r="I14">
-        <v>0.113324523809523</v>
+        <v>0.69086507936550001</v>
       </c>
       <c r="J14">
         <v>773</v>
@@ -1507,42 +1256,114 @@
         <v>150</v>
       </c>
       <c r="L14">
+        <f>(J14*K14)</f>
+        <v>115950</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15">
+        <v>0.58340000000000003</v>
+      </c>
+      <c r="F15">
+        <v>0.89229999999999998</v>
+      </c>
+      <c r="G15">
+        <v>0.94379999999999986</v>
+      </c>
+      <c r="H15">
+        <v>0.96689999999999987</v>
+      </c>
+      <c r="I15">
+        <v>0.76895473655000002</v>
+      </c>
+      <c r="J15">
+        <v>773</v>
+      </c>
+      <c r="K15">
+        <v>150</v>
+      </c>
+      <c r="L15">
+        <f t="shared" ref="L15:L17" si="2">(J15*K15)</f>
+        <v>115950</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16">
+        <v>0.54690000000000005</v>
+      </c>
+      <c r="F16">
+        <v>0.86450000000000005</v>
+      </c>
+      <c r="G16">
+        <v>0.92769999999999986</v>
+      </c>
+      <c r="H16">
+        <v>0.96349999999999991</v>
+      </c>
+      <c r="I16">
+        <v>0.73134650793651101</v>
+      </c>
+      <c r="J16">
+        <v>773</v>
+      </c>
+      <c r="K16">
+        <v>150</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="2"/>
         <v>115950</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15">
-        <v>4.6800000000000001E-2</v>
-      </c>
-      <c r="F15">
-        <v>0.1234</v>
-      </c>
-      <c r="G15">
-        <v>0.19220000000000001</v>
-      </c>
-      <c r="H15">
-        <v>0.35520000000000002</v>
-      </c>
-      <c r="I15">
-        <v>0.115741428571428</v>
-      </c>
-      <c r="J15">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17">
+        <v>0.62929999999999997</v>
+      </c>
+      <c r="F17">
+        <v>0.94850000000000001</v>
+      </c>
+      <c r="G17">
+        <v>0.97629999999999995</v>
+      </c>
+      <c r="H17">
+        <v>0.98350000000000004</v>
+      </c>
+      <c r="I17">
+        <v>0.78680865079365503</v>
+      </c>
+      <c r="J17">
         <v>773</v>
       </c>
-      <c r="K15">
+      <c r="K17">
         <v>150</v>
       </c>
-      <c r="L15">
+      <c r="L17">
         <f t="shared" si="2"/>
         <v>115950</v>
       </c>

</xml_diff>